<commit_message>
feat: Update topsis algorithm implementation and indicator formulas
</commit_message>
<xml_diff>
--- a/Repo/Articulo1/output/ranking_of_256_alternatives.xlsx
+++ b/Repo/Articulo1/output/ranking_of_256_alternatives.xlsx
@@ -470,7 +470,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>08/29/24</t>
+          <t>08/30/24</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -18697,7 +18697,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.7520669835929195</v>
+        <v>0.7501334446939418</v>
       </c>
     </row>
     <row r="3">
@@ -18705,7 +18705,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="n">
-        <v>0.7419426313801122</v>
+        <v>0.7417102541133376</v>
       </c>
     </row>
     <row r="4">
@@ -18713,7 +18713,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.7376032255725115</v>
+        <v>0.737129843364679</v>
       </c>
     </row>
     <row r="5">
@@ -18721,7 +18721,7 @@
         <v>9</v>
       </c>
       <c r="B5" t="n">
-        <v>0.7373558224938708</v>
+        <v>0.7343628323805469</v>
       </c>
     </row>
     <row r="6">
@@ -18729,7 +18729,7 @@
         <v>15</v>
       </c>
       <c r="B6" t="n">
-        <v>0.7322564285779858</v>
+        <v>0.7292325807785024</v>
       </c>
     </row>
     <row r="7">
@@ -18737,7 +18737,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="n">
-        <v>0.7308818904785781</v>
+        <v>0.7281483734140853</v>
       </c>
     </row>
     <row r="8">
@@ -18745,7 +18745,7 @@
         <v>26</v>
       </c>
       <c r="B8" t="n">
-        <v>0.7300929923918146</v>
+        <v>0.7269724153463858</v>
       </c>
     </row>
     <row r="9">
@@ -18753,7 +18753,7 @@
         <v>45</v>
       </c>
       <c r="B9" t="n">
-        <v>0.7173846064049632</v>
+        <v>0.7144108902790496</v>
       </c>
     </row>
     <row r="10">
@@ -18761,7 +18761,7 @@
         <v>71</v>
       </c>
       <c r="B10" t="n">
-        <v>0.7075475060370087</v>
+        <v>0.7046156405058827</v>
       </c>
     </row>
     <row r="11">
@@ -18769,7 +18769,7 @@
         <v>8</v>
       </c>
       <c r="B11" t="n">
-        <v>0.6904031170755346</v>
+        <v>0.6891961971777285</v>
       </c>
     </row>
     <row r="12">
@@ -18777,7 +18777,7 @@
         <v>102</v>
       </c>
       <c r="B12" t="n">
-        <v>0.6902482538099973</v>
+        <v>0.6875516021543341</v>
       </c>
     </row>
     <row r="13">
@@ -18785,7 +18785,7 @@
         <v>25</v>
       </c>
       <c r="B13" t="n">
-        <v>0.6866021429513069</v>
+        <v>0.6854523248295538</v>
       </c>
     </row>
     <row r="14">
@@ -18793,7 +18793,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="n">
-        <v>0.6835115041093401</v>
+        <v>0.6822871795423344</v>
       </c>
     </row>
     <row r="15">
@@ -18801,23 +18801,23 @@
         <v>24</v>
       </c>
       <c r="B15" t="n">
-        <v>0.679892878299704</v>
+        <v>0.6787496617819456</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>142</v>
+        <v>4</v>
       </c>
       <c r="B16" t="n">
-        <v>0.6760916909055812</v>
+        <v>0.6738015127490707</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>4</v>
+        <v>142</v>
       </c>
       <c r="B17" t="n">
-        <v>0.6743156429195106</v>
+        <v>0.6734605233100353</v>
       </c>
     </row>
     <row r="18">
@@ -18825,7 +18825,7 @@
         <v>44</v>
       </c>
       <c r="B18" t="n">
-        <v>0.6731421601854014</v>
+        <v>0.6720333146539674</v>
       </c>
     </row>
     <row r="19">
@@ -18833,23 +18833,23 @@
         <v>1</v>
       </c>
       <c r="B19" t="n">
-        <v>0.6710931733612077</v>
+        <v>0.670401432921659</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>70</v>
+        <v>13</v>
       </c>
       <c r="B20" t="n">
-        <v>0.6697810969169514</v>
+        <v>0.6695031892810187</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>13</v>
+        <v>70</v>
       </c>
       <c r="B21" t="n">
-        <v>0.6689571082411478</v>
+        <v>0.6688311138174718</v>
       </c>
     </row>
     <row r="22">
@@ -18857,7 +18857,7 @@
         <v>16</v>
       </c>
       <c r="B22" t="n">
-        <v>0.6683039113222652</v>
+        <v>0.6680687008598748</v>
       </c>
     </row>
     <row r="23">
@@ -18865,7 +18865,7 @@
         <v>10</v>
       </c>
       <c r="B23" t="n">
-        <v>0.6677571666700218</v>
+        <v>0.6672505309184418</v>
       </c>
     </row>
     <row r="24">
@@ -18873,23 +18873,23 @@
         <v>43</v>
       </c>
       <c r="B24" t="n">
-        <v>0.6661851425586081</v>
+        <v>0.6650818730540693</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>69</v>
+        <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>0.662796198101135</v>
+        <v>0.6633145853396308</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="B26" t="n">
-        <v>0.6624869583455836</v>
+        <v>0.6618517595132714</v>
       </c>
     </row>
     <row r="27">
@@ -18897,7 +18897,7 @@
         <v>27</v>
       </c>
       <c r="B27" t="n">
-        <v>0.6601926067969999</v>
+        <v>0.6599638751870088</v>
       </c>
     </row>
     <row r="28">
@@ -18905,7 +18905,7 @@
         <v>46</v>
       </c>
       <c r="B28" t="n">
-        <v>0.6579987113292254</v>
+        <v>0.6581817396291638</v>
       </c>
     </row>
     <row r="29">
@@ -18913,7 +18913,7 @@
         <v>193</v>
       </c>
       <c r="B29" t="n">
-        <v>0.6578773570423847</v>
+        <v>0.6554834709537098</v>
       </c>
     </row>
     <row r="30">
@@ -18921,7 +18921,7 @@
         <v>101</v>
       </c>
       <c r="B30" t="n">
-        <v>0.6519172517200634</v>
+        <v>0.6510343727446333</v>
       </c>
     </row>
     <row r="31">
@@ -18929,31 +18929,31 @@
         <v>72</v>
       </c>
       <c r="B31" t="n">
-        <v>0.6488701060247473</v>
+        <v>0.6490463515607182</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B32" t="n">
-        <v>0.6449126729439323</v>
+        <v>0.6444751062159868</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>141</v>
+        <v>100</v>
       </c>
       <c r="B33" t="n">
-        <v>0.6445272335425768</v>
+        <v>0.644033357649002</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>103</v>
+        <v>141</v>
       </c>
       <c r="B34" t="n">
-        <v>0.6436137280771536</v>
+        <v>0.6438464387277217</v>
       </c>
     </row>
     <row r="35">
@@ -18961,7 +18961,7 @@
         <v>255</v>
       </c>
       <c r="B35" t="n">
-        <v>0.6417467163625353</v>
+        <v>0.6393498807664626</v>
       </c>
     </row>
     <row r="36">
@@ -18969,7 +18969,7 @@
         <v>140</v>
       </c>
       <c r="B36" t="n">
-        <v>0.6377441372530408</v>
+        <v>0.6370659818152822</v>
       </c>
     </row>
     <row r="37">
@@ -18977,111 +18977,111 @@
         <v>143</v>
       </c>
       <c r="B37" t="n">
-        <v>0.6341228731801242</v>
+        <v>0.6349475772399689</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>6</v>
+        <v>194</v>
       </c>
       <c r="B38" t="n">
-        <v>0.6261490084375146</v>
+        <v>0.6253131057784228</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>192</v>
+        <v>5</v>
       </c>
       <c r="B39" t="n">
-        <v>0.6255562786243044</v>
+        <v>0.6249637588844582</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>19</v>
+        <v>192</v>
       </c>
       <c r="B40" t="n">
-        <v>0.6247656480215318</v>
+        <v>0.6249343016266201</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B41" t="n">
-        <v>0.6246218437725025</v>
+        <v>0.6248110712245233</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B42" t="n">
-        <v>0.6234480923521885</v>
+        <v>0.6233864222906085</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>194</v>
+        <v>22</v>
       </c>
       <c r="B43" t="n">
-        <v>0.6229991044240001</v>
+        <v>0.6220340768375044</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B44" t="n">
-        <v>0.6199496587718704</v>
+        <v>0.6207202393055685</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="B45" t="n">
-        <v>0.6199255282219633</v>
+        <v>0.6186357028449908</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="B46" t="n">
-        <v>0.6197463280048531</v>
+        <v>0.6185354401919956</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>54</v>
+        <v>191</v>
       </c>
       <c r="B47" t="n">
-        <v>0.6196329718689738</v>
+        <v>0.6182992664350002</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>191</v>
+        <v>54</v>
       </c>
       <c r="B48" t="n">
-        <v>0.6189200937172472</v>
+        <v>0.6182700042431721</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="B49" t="n">
-        <v>0.6181660718447565</v>
+        <v>0.6180940516189547</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>0.6174393723855951</v>
+        <v>0.6169245034025962</v>
       </c>
     </row>
     <row r="51">
@@ -19089,175 +19089,175 @@
         <v>254</v>
       </c>
       <c r="B51" t="n">
-        <v>0.6171014992192407</v>
+        <v>0.6166940924124784</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B52" t="n">
-        <v>0.6170997705711686</v>
+        <v>0.6157933977810067</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="B53" t="n">
-        <v>0.6169926802253008</v>
+        <v>0.6157336956526785</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="B54" t="n">
-        <v>0.6161204721658028</v>
+        <v>0.6156101043018782</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="B55" t="n">
-        <v>0.6159742288723937</v>
+        <v>0.6147677877449406</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B56" t="n">
-        <v>0.6151808461601176</v>
+        <v>0.6147118412558186</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="B57" t="n">
-        <v>0.6137438364195626</v>
+        <v>0.6146760663120732</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="B58" t="n">
-        <v>0.6128867991370011</v>
+        <v>0.6115170155874087</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>109</v>
+        <v>39</v>
       </c>
       <c r="B59" t="n">
-        <v>0.6121792688173459</v>
+        <v>0.6114660701309856</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>64</v>
+        <v>109</v>
       </c>
       <c r="B60" t="n">
-        <v>0.6120629345983258</v>
+        <v>0.6109357938185055</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>106</v>
+        <v>64</v>
       </c>
       <c r="B61" t="n">
-        <v>0.6117463745511951</v>
+        <v>0.6106922096327042</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>11</v>
+        <v>106</v>
       </c>
       <c r="B62" t="n">
-        <v>0.6111609079552521</v>
+        <v>0.6105594696274887</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>75</v>
+        <v>253</v>
       </c>
       <c r="B63" t="n">
-        <v>0.6109989502745347</v>
+        <v>0.610443826063238</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B64" t="n">
-        <v>0.6108740430989412</v>
+        <v>0.6097138234504522</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>253</v>
+        <v>78</v>
       </c>
       <c r="B65" t="n">
-        <v>0.6108506330005393</v>
+        <v>0.6095343834740669</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>113</v>
+        <v>30</v>
       </c>
       <c r="B66" t="n">
-        <v>0.6105055038759228</v>
+        <v>0.6094012609314717</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>30</v>
+        <v>104</v>
       </c>
       <c r="B67" t="n">
-        <v>0.608757741490129</v>
+        <v>0.6093366034374057</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>82</v>
+        <v>113</v>
       </c>
       <c r="B68" t="n">
-        <v>0.6086133485939772</v>
+        <v>0.609229531350015</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>104</v>
+        <v>195</v>
       </c>
       <c r="B69" t="n">
-        <v>0.6078577222807677</v>
+        <v>0.6084084423026405</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>119</v>
+        <v>82</v>
       </c>
       <c r="B70" t="n">
-        <v>0.6066451170475674</v>
+        <v>0.6072461799919319</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>195</v>
+        <v>119</v>
       </c>
       <c r="B71" t="n">
-        <v>0.6064514894123259</v>
+        <v>0.6053645164429282</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>88</v>
+        <v>144</v>
       </c>
       <c r="B72" t="n">
-        <v>0.6042019459932083</v>
+        <v>0.6050259939081301</v>
       </c>
     </row>
     <row r="73">
@@ -19265,71 +19265,71 @@
         <v>73</v>
       </c>
       <c r="B73" t="n">
-        <v>0.6039648643584773</v>
+        <v>0.6049588821532044</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
-        <v>144</v>
+        <v>88</v>
       </c>
       <c r="B74" t="n">
-        <v>0.6036765789219268</v>
+        <v>0.6028373712302456</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
-        <v>150</v>
+        <v>197</v>
       </c>
       <c r="B75" t="n">
-        <v>0.6024241308994239</v>
+        <v>0.6027578088251254</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B76" t="n">
-        <v>0.6019818270800209</v>
+        <v>0.6012157933058653</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
-        <v>202</v>
+        <v>147</v>
       </c>
       <c r="B77" t="n">
-        <v>0.6013891276237676</v>
+        <v>0.6008328157273594</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
-        <v>154</v>
+        <v>202</v>
       </c>
       <c r="B78" t="n">
-        <v>0.6009819326354277</v>
+        <v>0.6003359971721136</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
-        <v>126</v>
+        <v>154</v>
       </c>
       <c r="B79" t="n">
-        <v>0.60077121467551</v>
+        <v>0.5997355887088406</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B80" t="n">
-        <v>0.6006984127265478</v>
+        <v>0.599582187465188</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
-        <v>199</v>
+        <v>126</v>
       </c>
       <c r="B81" t="n">
-        <v>0.6005801657317789</v>
+        <v>0.5995137745975067</v>
       </c>
     </row>
     <row r="82">
@@ -19337,39 +19337,39 @@
         <v>206</v>
       </c>
       <c r="B82" t="n">
-        <v>0.6004192830283875</v>
+        <v>0.5993281927757944</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B83" t="n">
-        <v>0.5999353175459458</v>
+        <v>0.5988667250566556</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
-        <v>196</v>
+        <v>145</v>
       </c>
       <c r="B84" t="n">
-        <v>0.5982891059084643</v>
+        <v>0.5988606252592322</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
-        <v>95</v>
+        <v>196</v>
       </c>
       <c r="B85" t="n">
-        <v>0.5978762457069702</v>
+        <v>0.5973578847548973</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
-        <v>160</v>
+        <v>95</v>
       </c>
       <c r="B86" t="n">
-        <v>0.5975500718995224</v>
+        <v>0.5965432262028061</v>
       </c>
     </row>
     <row r="87">
@@ -19377,15 +19377,15 @@
         <v>212</v>
       </c>
       <c r="B87" t="n">
-        <v>0.5975243211672883</v>
+        <v>0.5964166551287929</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
-        <v>146</v>
+        <v>160</v>
       </c>
       <c r="B88" t="n">
-        <v>0.5974455437310467</v>
+        <v>0.5962913307254336</v>
       </c>
     </row>
     <row r="89">
@@ -19393,7 +19393,7 @@
         <v>134</v>
       </c>
       <c r="B89" t="n">
-        <v>0.5932816667808194</v>
+        <v>0.5920713940896997</v>
       </c>
     </row>
     <row r="90">
@@ -19401,7 +19401,7 @@
         <v>219</v>
       </c>
       <c r="B90" t="n">
-        <v>0.5927638284530008</v>
+        <v>0.5916625837598258</v>
       </c>
     </row>
     <row r="91">
@@ -19409,7 +19409,7 @@
         <v>167</v>
       </c>
       <c r="B91" t="n">
-        <v>0.5922465162629245</v>
+        <v>0.5910019847730954</v>
       </c>
     </row>
     <row r="92">
@@ -19417,23 +19417,23 @@
         <v>68</v>
       </c>
       <c r="B92" t="n">
-        <v>0.5864954715061534</v>
+        <v>0.5864526155592824</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
-        <v>226</v>
+        <v>42</v>
       </c>
       <c r="B93" t="n">
-        <v>0.5864073291809636</v>
+        <v>0.5861983259521213</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
-        <v>42</v>
+        <v>226</v>
       </c>
       <c r="B94" t="n">
-        <v>0.5863928928275902</v>
+        <v>0.5853341200243051</v>
       </c>
     </row>
     <row r="95">
@@ -19441,7 +19441,7 @@
         <v>175</v>
       </c>
       <c r="B95" t="n">
-        <v>0.5854008541932119</v>
+        <v>0.5841946476540661</v>
       </c>
     </row>
     <row r="96">
@@ -19449,31 +19449,31 @@
         <v>234</v>
       </c>
       <c r="B96" t="n">
-        <v>0.5788810200319434</v>
+        <v>0.577853638030821</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
-        <v>183</v>
+        <v>67</v>
       </c>
       <c r="B97" t="n">
-        <v>0.5774849206996929</v>
+        <v>0.5769287540452269</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="B98" t="n">
-        <v>0.5769710879985885</v>
+        <v>0.5766962654082906</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
-        <v>41</v>
+        <v>183</v>
       </c>
       <c r="B99" t="n">
-        <v>0.5768886643785299</v>
+        <v>0.5763361028819656</v>
       </c>
     </row>
     <row r="100">
@@ -19481,7 +19481,7 @@
         <v>99</v>
       </c>
       <c r="B100" t="n">
-        <v>0.5707597461525616</v>
+        <v>0.5707185056136299</v>
       </c>
     </row>
     <row r="101">
@@ -19489,7 +19489,7 @@
         <v>244</v>
       </c>
       <c r="B101" t="n">
-        <v>0.5706792893860836</v>
+        <v>0.5697104380685623</v>
       </c>
     </row>
     <row r="102">
@@ -19497,7 +19497,7 @@
         <v>139</v>
       </c>
       <c r="B102" t="n">
-        <v>0.5688500964443456</v>
+        <v>0.5689781017417522</v>
       </c>
     </row>
     <row r="103">
@@ -19505,7 +19505,7 @@
         <v>40</v>
       </c>
       <c r="B103" t="n">
-        <v>0.5644912972264796</v>
+        <v>0.5654836840798557</v>
       </c>
     </row>
     <row r="104">
@@ -19513,7 +19513,7 @@
         <v>98</v>
       </c>
       <c r="B104" t="n">
-        <v>0.5614227953490484</v>
+        <v>0.5613819418842549</v>
       </c>
     </row>
     <row r="105">
@@ -19521,23 +19521,23 @@
         <v>138</v>
       </c>
       <c r="B105" t="n">
-        <v>0.5598343366762307</v>
+        <v>0.5599611116459918</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
-        <v>18</v>
+        <v>65</v>
       </c>
       <c r="B106" t="n">
-        <v>0.5557899137547269</v>
+        <v>0.5563865261186118</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
-        <v>65</v>
+        <v>18</v>
       </c>
       <c r="B107" t="n">
-        <v>0.5551908438558648</v>
+        <v>0.5554453472512338</v>
       </c>
     </row>
     <row r="108">
@@ -19545,7 +19545,7 @@
         <v>190</v>
       </c>
       <c r="B108" t="n">
-        <v>0.5528924007053005</v>
+        <v>0.5530130092236463</v>
       </c>
     </row>
     <row r="109">
@@ -19553,7 +19553,7 @@
         <v>50</v>
       </c>
       <c r="B109" t="n">
-        <v>0.5528886369642084</v>
+        <v>0.5526770712308583</v>
       </c>
     </row>
     <row r="110">
@@ -19561,7 +19561,7 @@
         <v>21</v>
       </c>
       <c r="B110" t="n">
-        <v>0.5527562141919371</v>
+        <v>0.5524016063048911</v>
       </c>
     </row>
     <row r="111">
@@ -19569,7 +19569,7 @@
         <v>252</v>
       </c>
       <c r="B111" t="n">
-        <v>0.5505661471287916</v>
+        <v>0.5508594974973121</v>
       </c>
     </row>
     <row r="112">
@@ -19577,7 +19577,7 @@
         <v>53</v>
       </c>
       <c r="B112" t="n">
-        <v>0.550171043923484</v>
+        <v>0.5499510745035412</v>
       </c>
     </row>
     <row r="113">
@@ -19585,7 +19585,7 @@
         <v>105</v>
       </c>
       <c r="B113" t="n">
-        <v>0.5488144504371277</v>
+        <v>0.5487760327776342</v>
       </c>
     </row>
     <row r="114">
@@ -19593,7 +19593,7 @@
         <v>31</v>
       </c>
       <c r="B114" t="n">
-        <v>0.5478369257241182</v>
+        <v>0.5474924903786582</v>
       </c>
     </row>
     <row r="115">
@@ -19601,7 +19601,7 @@
         <v>108</v>
       </c>
       <c r="B115" t="n">
-        <v>0.5463790025776786</v>
+        <v>0.546338683524012</v>
       </c>
     </row>
     <row r="116">
@@ -19609,39 +19609,39 @@
         <v>57</v>
       </c>
       <c r="B116" t="n">
-        <v>0.5463351880277317</v>
+        <v>0.5461105053538976</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
-        <v>34</v>
+        <v>189</v>
       </c>
       <c r="B117" t="n">
-        <v>0.5447407751117197</v>
+        <v>0.5443996935226891</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
-        <v>74</v>
+        <v>34</v>
       </c>
       <c r="B118" t="n">
-        <v>0.5443022124027863</v>
+        <v>0.5443844233469091</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="B119" t="n">
-        <v>0.5442799048245338</v>
+        <v>0.5441190575108881</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
-        <v>198</v>
+        <v>74</v>
       </c>
       <c r="B120" t="n">
-        <v>0.5439441530718137</v>
+        <v>0.5440929802302981</v>
       </c>
     </row>
     <row r="121">
@@ -19649,7 +19649,7 @@
         <v>112</v>
       </c>
       <c r="B121" t="n">
-        <v>0.542857410025156</v>
+        <v>0.5428158090201617</v>
       </c>
     </row>
     <row r="122">
@@ -19657,7 +19657,7 @@
         <v>251</v>
       </c>
       <c r="B122" t="n">
-        <v>0.5424939360108004</v>
+        <v>0.5427852931209879</v>
       </c>
     </row>
     <row r="123">
@@ -19665,7 +19665,7 @@
         <v>201</v>
       </c>
       <c r="B123" t="n">
-        <v>0.5417258708872233</v>
+        <v>0.5419108578774101</v>
       </c>
     </row>
     <row r="124">
@@ -19673,7 +19673,7 @@
         <v>63</v>
       </c>
       <c r="B124" t="n">
-        <v>0.5415180037528655</v>
+        <v>0.5412927468311111</v>
       </c>
     </row>
     <row r="125">
@@ -19681,7 +19681,7 @@
         <v>77</v>
       </c>
       <c r="B125" t="n">
-        <v>0.5414366424896853</v>
+        <v>0.5412180304469466</v>
       </c>
     </row>
     <row r="126">
@@ -19689,7 +19689,7 @@
         <v>38</v>
       </c>
       <c r="B126" t="n">
-        <v>0.5406535555928139</v>
+        <v>0.5402912657234176</v>
       </c>
     </row>
     <row r="127">
@@ -19697,7 +19697,7 @@
         <v>205</v>
       </c>
       <c r="B127" t="n">
-        <v>0.5385030180007058</v>
+        <v>0.5386956224424452</v>
       </c>
     </row>
     <row r="128">
@@ -19705,7 +19705,7 @@
         <v>118</v>
       </c>
       <c r="B128" t="n">
-        <v>0.5383409326150927</v>
+        <v>0.5382987937969075</v>
       </c>
     </row>
     <row r="129">
@@ -19713,7 +19713,7 @@
         <v>56</v>
       </c>
       <c r="B129" t="n">
-        <v>0.5376413460962387</v>
+        <v>0.5374144109103732</v>
       </c>
     </row>
     <row r="130">
@@ -19721,39 +19721,39 @@
         <v>81</v>
       </c>
       <c r="B130" t="n">
-        <v>0.5375745354700538</v>
+        <v>0.5373499980884712</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="n">
-        <v>149</v>
+        <v>20</v>
       </c>
       <c r="B131" t="n">
-        <v>0.5372226322274808</v>
+        <v>0.537329027562634</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="n">
-        <v>20</v>
+        <v>149</v>
       </c>
       <c r="B132" t="n">
-        <v>0.536397368434434</v>
+        <v>0.5371829910945292</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="n">
-        <v>211</v>
+        <v>52</v>
       </c>
       <c r="B133" t="n">
-        <v>0.5343273122346746</v>
+        <v>0.535245569533419</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="n">
-        <v>52</v>
+        <v>211</v>
       </c>
       <c r="B134" t="n">
-        <v>0.5340304069711624</v>
+        <v>0.5345243576859233</v>
       </c>
     </row>
     <row r="135">
@@ -19761,7 +19761,7 @@
         <v>111</v>
       </c>
       <c r="B135" t="n">
-        <v>0.533771842933915</v>
+        <v>0.5337301052443731</v>
       </c>
     </row>
     <row r="136">
@@ -19769,7 +19769,7 @@
         <v>153</v>
       </c>
       <c r="B136" t="n">
-        <v>0.5335965053399176</v>
+        <v>0.5335553950685884</v>
       </c>
     </row>
     <row r="137">
@@ -19777,95 +19777,95 @@
         <v>125</v>
       </c>
       <c r="B137" t="n">
-        <v>0.5330423543369018</v>
+        <v>0.5330004702083876</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="1" t="n">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="B138" t="n">
-        <v>0.532847626445018</v>
+        <v>0.5327378240238058</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="n">
-        <v>62</v>
+        <v>87</v>
       </c>
       <c r="B139" t="n">
-        <v>0.5327954564050001</v>
+        <v>0.5326211879186268</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="1" t="n">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="B140" t="n">
-        <v>0.532178932438331</v>
+        <v>0.5325670676075402</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="1" t="n">
-        <v>107</v>
+        <v>37</v>
       </c>
       <c r="B141" t="n">
-        <v>0.5312086168052358</v>
+        <v>0.5318113340496283</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="1" t="n">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="B142" t="n">
-        <v>0.5293657246324333</v>
+        <v>0.5301826427867783</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="n">
-        <v>204</v>
+        <v>218</v>
       </c>
       <c r="B143" t="n">
-        <v>0.5293300282745922</v>
+        <v>0.5295636056735473</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="1" t="n">
-        <v>117</v>
+        <v>204</v>
       </c>
       <c r="B144" t="n">
-        <v>0.5291594763450932</v>
+        <v>0.5295220209393748</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="1" t="n">
-        <v>159</v>
+        <v>117</v>
       </c>
       <c r="B145" t="n">
-        <v>0.5291119870317488</v>
+        <v>0.5291170352550013</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="1" t="n">
-        <v>80</v>
+        <v>159</v>
       </c>
       <c r="B146" t="n">
-        <v>0.5286072999698195</v>
+        <v>0.5290701052186588</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="1" t="n">
-        <v>200</v>
+        <v>33</v>
       </c>
       <c r="B147" t="n">
-        <v>0.5283109481264618</v>
+        <v>0.5289432591962557</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="1" t="n">
-        <v>33</v>
+        <v>80</v>
       </c>
       <c r="B148" t="n">
-        <v>0.5280107532280597</v>
+        <v>0.5283809331057855</v>
       </c>
     </row>
     <row r="149">
@@ -19873,7 +19873,7 @@
         <v>94</v>
       </c>
       <c r="B149" t="n">
-        <v>0.5274938757236892</v>
+        <v>0.5272697149425613</v>
       </c>
     </row>
     <row r="150">
@@ -19881,7 +19881,7 @@
         <v>133</v>
       </c>
       <c r="B150" t="n">
-        <v>0.5272646466113967</v>
+        <v>0.5272237716778837</v>
       </c>
     </row>
     <row r="151">
@@ -19889,7 +19889,7 @@
         <v>76</v>
       </c>
       <c r="B151" t="n">
-        <v>0.5252469099766619</v>
+        <v>0.5264500815964995</v>
       </c>
     </row>
     <row r="152">
@@ -19897,7 +19897,7 @@
         <v>210</v>
       </c>
       <c r="B152" t="n">
-        <v>0.5249878109628926</v>
+        <v>0.5251849476862031</v>
       </c>
     </row>
     <row r="153">
@@ -19905,47 +19905,47 @@
         <v>152</v>
       </c>
       <c r="B153" t="n">
-        <v>0.5244135154750107</v>
+        <v>0.52437234045536</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="1" t="n">
-        <v>166</v>
+        <v>225</v>
       </c>
       <c r="B154" t="n">
-        <v>0.5239720671499321</v>
+        <v>0.5240777453893365</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="1" t="n">
-        <v>124</v>
+        <v>166</v>
       </c>
       <c r="B155" t="n">
-        <v>0.5239002286781618</v>
+        <v>0.5239301854408722</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="1" t="n">
-        <v>225</v>
+        <v>124</v>
       </c>
       <c r="B156" t="n">
-        <v>0.5238826828395476</v>
+        <v>0.523857878504032</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="1" t="n">
-        <v>86</v>
+        <v>148</v>
       </c>
       <c r="B157" t="n">
-        <v>0.5237911010554477</v>
+        <v>0.5238242730325869</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="1" t="n">
-        <v>148</v>
+        <v>86</v>
       </c>
       <c r="B158" t="n">
-        <v>0.5223256696882205</v>
+        <v>0.5235619273670452</v>
       </c>
     </row>
     <row r="159">
@@ -19953,7 +19953,7 @@
         <v>55</v>
       </c>
       <c r="B159" t="n">
-        <v>0.5207773242337954</v>
+        <v>0.5220204586363482</v>
       </c>
     </row>
     <row r="160">
@@ -19961,7 +19961,7 @@
         <v>217</v>
       </c>
       <c r="B160" t="n">
-        <v>0.5200003590651957</v>
+        <v>0.5201991049475617</v>
       </c>
     </row>
     <row r="161">
@@ -19969,15 +19969,15 @@
         <v>158</v>
       </c>
       <c r="B161" t="n">
-        <v>0.5197688640822437</v>
+        <v>0.5197267552582415</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="1" t="n">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="B162" t="n">
-        <v>0.5184780050329649</v>
+        <v>0.51968300984982</v>
       </c>
     </row>
     <row r="163">
@@ -19985,31 +19985,31 @@
         <v>174</v>
       </c>
       <c r="B163" t="n">
-        <v>0.5184606879259163</v>
+        <v>0.5184195703693825</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="1" t="n">
-        <v>132</v>
+        <v>233</v>
       </c>
       <c r="B164" t="n">
-        <v>0.5182912732525208</v>
+        <v>0.5183836803951557</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="1" t="n">
-        <v>233</v>
+        <v>93</v>
       </c>
       <c r="B165" t="n">
-        <v>0.5181947571999518</v>
+        <v>0.5182502746491418</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="1" t="n">
-        <v>110</v>
+        <v>132</v>
       </c>
       <c r="B166" t="n">
-        <v>0.5181144486852947</v>
+        <v>0.518249790513012</v>
       </c>
     </row>
     <row r="167">
@@ -20017,7 +20017,7 @@
         <v>203</v>
       </c>
       <c r="B167" t="n">
-        <v>0.5157101539490554</v>
+        <v>0.5176334601179395</v>
       </c>
     </row>
     <row r="168">
@@ -20025,7 +20025,7 @@
         <v>36</v>
       </c>
       <c r="B168" t="n">
-        <v>0.5146720499436256</v>
+        <v>0.5156266424965209</v>
       </c>
     </row>
     <row r="169">
@@ -20033,7 +20033,7 @@
         <v>224</v>
       </c>
       <c r="B169" t="n">
-        <v>0.5146316943024861</v>
+        <v>0.514828371900251</v>
       </c>
     </row>
     <row r="170">
@@ -20041,55 +20041,55 @@
         <v>165</v>
       </c>
       <c r="B170" t="n">
-        <v>0.5146075812957984</v>
+        <v>0.5145653063238819</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="1" t="n">
-        <v>182</v>
+        <v>79</v>
       </c>
       <c r="B171" t="n">
-        <v>0.5128924259678769</v>
+        <v>0.5130752777533514</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="1" t="n">
-        <v>243</v>
+        <v>182</v>
       </c>
       <c r="B172" t="n">
-        <v>0.5126133619617345</v>
+        <v>0.5128527512951412</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="1" t="n">
-        <v>79</v>
+        <v>243</v>
       </c>
       <c r="B173" t="n">
-        <v>0.5118398195803028</v>
+        <v>0.5127934494771312</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="1" t="n">
-        <v>173</v>
+        <v>151</v>
       </c>
       <c r="B174" t="n">
-        <v>0.5092138685231866</v>
+        <v>0.5107364839718512</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="1" t="n">
-        <v>151</v>
+        <v>232</v>
       </c>
       <c r="B175" t="n">
-        <v>0.509194131377504</v>
+        <v>0.5093781201829234</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="1" t="n">
-        <v>232</v>
+        <v>173</v>
       </c>
       <c r="B176" t="n">
-        <v>0.5091869451642314</v>
+        <v>0.5091722078805722</v>
       </c>
     </row>
     <row r="177">
@@ -20097,7 +20097,7 @@
         <v>242</v>
       </c>
       <c r="B177" t="n">
-        <v>0.5039576314414866</v>
+        <v>0.5041404324427202</v>
       </c>
     </row>
     <row r="178">
@@ -20105,7 +20105,7 @@
         <v>181</v>
       </c>
       <c r="B178" t="n">
-        <v>0.5038918828356761</v>
+        <v>0.5038515488814621</v>
       </c>
     </row>
     <row r="179">
@@ -20113,7 +20113,7 @@
         <v>66</v>
       </c>
       <c r="B179" t="n">
-        <v>0.4916124866851519</v>
+        <v>0.4919827796545825</v>
       </c>
     </row>
     <row r="180">
@@ -20121,7 +20121,7 @@
         <v>137</v>
       </c>
       <c r="B180" t="n">
-        <v>0.4790723962481566</v>
+        <v>0.4795854899677941</v>
       </c>
     </row>
     <row r="181">
@@ -20129,7 +20129,7 @@
         <v>97</v>
       </c>
       <c r="B181" t="n">
-        <v>0.4778077334832291</v>
+        <v>0.4781758835522625</v>
       </c>
     </row>
     <row r="182">
@@ -20137,7 +20137,7 @@
         <v>136</v>
       </c>
       <c r="B182" t="n">
-        <v>0.470431125669326</v>
+        <v>0.4709403415094777</v>
       </c>
     </row>
     <row r="183">
@@ -20145,7 +20145,7 @@
         <v>250</v>
       </c>
       <c r="B183" t="n">
-        <v>0.4694324148381674</v>
+        <v>0.4700682582404903</v>
       </c>
     </row>
     <row r="184">
@@ -20153,7 +20153,7 @@
         <v>188</v>
       </c>
       <c r="B184" t="n">
-        <v>0.466743130579259</v>
+        <v>0.4672407704402434</v>
       </c>
     </row>
     <row r="185">
@@ -20161,7 +20161,7 @@
         <v>249</v>
       </c>
       <c r="B185" t="n">
-        <v>0.4616678111860799</v>
+        <v>0.4622992826408316</v>
       </c>
     </row>
     <row r="186">
@@ -20169,7 +20169,7 @@
         <v>96</v>
       </c>
       <c r="B186" t="n">
-        <v>0.459638783153791</v>
+        <v>0.4608905894178772</v>
       </c>
     </row>
     <row r="187">
@@ -20177,7 +20177,7 @@
         <v>187</v>
       </c>
       <c r="B187" t="n">
-        <v>0.4585357952735477</v>
+        <v>0.4590305391915497</v>
       </c>
     </row>
     <row r="188">
@@ -20185,7 +20185,7 @@
         <v>135</v>
       </c>
       <c r="B188" t="n">
-        <v>0.4545883737509753</v>
+        <v>0.4559856425356057</v>
       </c>
     </row>
     <row r="189">
@@ -20193,7 +20193,7 @@
         <v>61</v>
       </c>
       <c r="B189" t="n">
-        <v>0.4536189542269509</v>
+        <v>0.4539084701978784</v>
       </c>
     </row>
     <row r="190">
@@ -20201,7 +20201,7 @@
         <v>116</v>
       </c>
       <c r="B190" t="n">
-        <v>0.4489830581926208</v>
+        <v>0.4494597264742093</v>
       </c>
     </row>
     <row r="191">
@@ -20209,7 +20209,7 @@
         <v>209</v>
       </c>
       <c r="B191" t="n">
-        <v>0.4459020859849816</v>
+        <v>0.446593086212351</v>
       </c>
     </row>
     <row r="192">
@@ -20217,7 +20217,7 @@
         <v>85</v>
       </c>
       <c r="B192" t="n">
-        <v>0.4444579311053922</v>
+        <v>0.4447522928811696</v>
       </c>
     </row>
     <row r="193">
@@ -20225,7 +20225,7 @@
         <v>60</v>
       </c>
       <c r="B193" t="n">
-        <v>0.4442451886154591</v>
+        <v>0.4445390427122103</v>
       </c>
     </row>
     <row r="194">
@@ -20233,7 +20233,7 @@
         <v>123</v>
       </c>
       <c r="B194" t="n">
-        <v>0.4436353927686107</v>
+        <v>0.4441171292387829</v>
       </c>
     </row>
     <row r="195">
@@ -20241,7 +20241,7 @@
         <v>157</v>
       </c>
       <c r="B195" t="n">
-        <v>0.44023400359575</v>
+        <v>0.4407134487830057</v>
       </c>
     </row>
     <row r="196">
@@ -20249,7 +20249,7 @@
         <v>216</v>
       </c>
       <c r="B196" t="n">
-        <v>0.4399785186946585</v>
+        <v>0.4406841660130292</v>
       </c>
     </row>
     <row r="197">
@@ -20257,87 +20257,87 @@
         <v>115</v>
       </c>
       <c r="B197" t="n">
-        <v>0.4397622615844604</v>
+        <v>0.440243103889187</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="1" t="n">
-        <v>92</v>
+        <v>131</v>
       </c>
       <c r="B198" t="n">
-        <v>0.4394326262479731</v>
+        <v>0.4398291248953278</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="1" t="n">
-        <v>131</v>
+        <v>92</v>
       </c>
       <c r="B199" t="n">
-        <v>0.4393514164596579</v>
+        <v>0.4397287914121339</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="1" t="n">
-        <v>208</v>
+        <v>59</v>
       </c>
       <c r="B200" t="n">
-        <v>0.4371477056693854</v>
+        <v>0.4383150687646045</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="1" t="n">
-        <v>59</v>
+        <v>208</v>
       </c>
       <c r="B201" t="n">
-        <v>0.4369794262549716</v>
+        <v>0.4378399135444996</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="1" t="n">
-        <v>84</v>
+        <v>223</v>
       </c>
       <c r="B202" t="n">
-        <v>0.4351159591422762</v>
+        <v>0.4357988710274517</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="1" t="n">
-        <v>223</v>
+        <v>114</v>
       </c>
       <c r="B203" t="n">
-        <v>0.4350918121040857</v>
+        <v>0.4354510826873431</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="1" t="n">
-        <v>164</v>
+        <v>84</v>
       </c>
       <c r="B204" t="n">
-        <v>0.4345079115367863</v>
+        <v>0.4354142976569494</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="1" t="n">
-        <v>122</v>
+        <v>164</v>
       </c>
       <c r="B205" t="n">
-        <v>0.434151574904914</v>
+        <v>0.4349955023793463</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="1" t="n">
-        <v>114</v>
+        <v>207</v>
       </c>
       <c r="B206" t="n">
-        <v>0.4338403028810084</v>
+        <v>0.4347643206164366</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="1" t="n">
-        <v>207</v>
+        <v>122</v>
       </c>
       <c r="B207" t="n">
-        <v>0.4328778344942845</v>
+        <v>0.4346395621433395</v>
       </c>
     </row>
     <row r="208">
@@ -20345,7 +20345,7 @@
         <v>231</v>
       </c>
       <c r="B208" t="n">
-        <v>0.4315087090602681</v>
+        <v>0.4322035096259269</v>
       </c>
     </row>
     <row r="209">
@@ -20353,7 +20353,7 @@
         <v>156</v>
       </c>
       <c r="B209" t="n">
-        <v>0.4312289566043352</v>
+        <v>0.4317116839718054</v>
       </c>
     </row>
     <row r="210">
@@ -20361,7 +20361,7 @@
         <v>215</v>
       </c>
       <c r="B210" t="n">
-        <v>0.4309091258342969</v>
+        <v>0.4316189862624723</v>
       </c>
     </row>
     <row r="211">
@@ -20369,23 +20369,23 @@
         <v>172</v>
       </c>
       <c r="B211" t="n">
-        <v>0.4299703569215543</v>
+        <v>0.4304567388245525</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="1" t="n">
-        <v>91</v>
+        <v>130</v>
       </c>
       <c r="B212" t="n">
-        <v>0.4298406328718496</v>
+        <v>0.4302440033623776</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="1" t="n">
-        <v>130</v>
+        <v>91</v>
       </c>
       <c r="B213" t="n">
-        <v>0.4297582864027949</v>
+        <v>0.4301420292108027</v>
       </c>
     </row>
     <row r="214">
@@ -20393,7 +20393,7 @@
         <v>241</v>
       </c>
       <c r="B214" t="n">
-        <v>0.429346684286974</v>
+        <v>0.4300167160554416</v>
       </c>
     </row>
     <row r="215">
@@ -20401,23 +20401,23 @@
         <v>83</v>
       </c>
       <c r="B215" t="n">
-        <v>0.4283856210992566</v>
+        <v>0.4297377872649712</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="1" t="n">
-        <v>180</v>
+        <v>155</v>
       </c>
       <c r="B216" t="n">
-        <v>0.426851007826844</v>
+        <v>0.427587282117785</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="1" t="n">
-        <v>155</v>
+        <v>180</v>
       </c>
       <c r="B217" t="n">
-        <v>0.425974878558167</v>
+        <v>0.4273267717001381</v>
       </c>
     </row>
     <row r="218">
@@ -20425,7 +20425,7 @@
         <v>222</v>
       </c>
       <c r="B218" t="n">
-        <v>0.4258368749146296</v>
+        <v>0.4265510113560076</v>
       </c>
     </row>
     <row r="219">
@@ -20433,7 +20433,7 @@
         <v>163</v>
       </c>
       <c r="B219" t="n">
-        <v>0.425181031030446</v>
+        <v>0.4256740874854273</v>
       </c>
     </row>
     <row r="220">
@@ -20441,39 +20441,39 @@
         <v>230</v>
       </c>
       <c r="B220" t="n">
-        <v>0.4222221991117669</v>
+        <v>0.4229264173435436</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="n">
-        <v>171</v>
+        <v>120</v>
       </c>
       <c r="B221" t="n">
-        <v>0.4204662046345685</v>
+        <v>0.4220498966555591</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="1" t="n">
-        <v>120</v>
+        <v>213</v>
       </c>
       <c r="B222" t="n">
-        <v>0.42041594240448</v>
+        <v>0.4214465799872265</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="n">
-        <v>240</v>
+        <v>171</v>
       </c>
       <c r="B223" t="n">
-        <v>0.4201909934611895</v>
+        <v>0.4209599855007634</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="n">
-        <v>213</v>
+        <v>240</v>
       </c>
       <c r="B224" t="n">
-        <v>0.4195285929151994</v>
+        <v>0.4208719973468465</v>
       </c>
     </row>
     <row r="225">
@@ -20481,7 +20481,7 @@
         <v>179</v>
       </c>
       <c r="B225" t="n">
-        <v>0.417338576859405</v>
+        <v>0.417823163237815</v>
       </c>
     </row>
     <row r="226">
@@ -20489,7 +20489,7 @@
         <v>89</v>
       </c>
       <c r="B226" t="n">
-        <v>0.4150747305196018</v>
+        <v>0.416447170140784</v>
       </c>
     </row>
     <row r="227">
@@ -20497,7 +20497,7 @@
         <v>161</v>
       </c>
       <c r="B227" t="n">
-        <v>0.4124929728995921</v>
+        <v>0.4141346405593411</v>
       </c>
     </row>
     <row r="228">
@@ -20505,7 +20505,7 @@
         <v>248</v>
       </c>
       <c r="B228" t="n">
-        <v>0.3916545123571975</v>
+        <v>0.3925220873773694</v>
       </c>
     </row>
     <row r="229">
@@ -20513,7 +20513,7 @@
         <v>186</v>
       </c>
       <c r="B229" t="n">
-        <v>0.3865913939758068</v>
+        <v>0.3873431357626024</v>
       </c>
     </row>
     <row r="230">
@@ -20521,23 +20521,23 @@
         <v>247</v>
       </c>
       <c r="B230" t="n">
-        <v>0.3863331406166964</v>
+        <v>0.3871902622638588</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="n">
-        <v>185</v>
+        <v>245</v>
       </c>
       <c r="B231" t="n">
-        <v>0.3810440440574939</v>
+        <v>0.3821740992849041</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="n">
-        <v>245</v>
+        <v>185</v>
       </c>
       <c r="B232" t="n">
-        <v>0.3806575114710931</v>
+        <v>0.3817875314993371</v>
       </c>
     </row>
     <row r="233">
@@ -20545,7 +20545,7 @@
         <v>184</v>
       </c>
       <c r="B233" t="n">
-        <v>0.3781739809116028</v>
+        <v>0.3796191624113534</v>
       </c>
     </row>
     <row r="234">
@@ -20553,7 +20553,7 @@
         <v>121</v>
       </c>
       <c r="B234" t="n">
-        <v>0.3664435736371561</v>
+        <v>0.3672328570271651</v>
       </c>
     </row>
     <row r="235">
@@ -20561,7 +20561,7 @@
         <v>90</v>
       </c>
       <c r="B235" t="n">
-        <v>0.3649084449900614</v>
+        <v>0.3655184811846721</v>
       </c>
     </row>
     <row r="236">
@@ -20569,7 +20569,7 @@
         <v>129</v>
       </c>
       <c r="B236" t="n">
-        <v>0.3624174058101221</v>
+        <v>0.3632106122535265</v>
       </c>
     </row>
     <row r="237">
@@ -20577,7 +20577,7 @@
         <v>214</v>
       </c>
       <c r="B237" t="n">
-        <v>0.361985305154603</v>
+        <v>0.3629863675452126</v>
       </c>
     </row>
     <row r="238">
@@ -20585,7 +20585,7 @@
         <v>162</v>
       </c>
       <c r="B238" t="n">
-        <v>0.3581888552705149</v>
+        <v>0.3589938208042283</v>
       </c>
     </row>
     <row r="239">
@@ -20593,7 +20593,7 @@
         <v>221</v>
       </c>
       <c r="B239" t="n">
-        <v>0.3565851480389581</v>
+        <v>0.357604156790503</v>
       </c>
     </row>
     <row r="240">
@@ -20601,31 +20601,31 @@
         <v>128</v>
       </c>
       <c r="B240" t="n">
-        <v>0.3548841326147224</v>
+        <v>0.3556867087088774</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="n">
-        <v>229</v>
+        <v>127</v>
       </c>
       <c r="B241" t="n">
-        <v>0.3538104609838379</v>
+        <v>0.3553970977533982</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="n">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="B242" t="n">
-        <v>0.3537386994577829</v>
+        <v>0.3548232706706828</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="n">
-        <v>127</v>
+        <v>239</v>
       </c>
       <c r="B243" t="n">
-        <v>0.3537243114324256</v>
+        <v>0.3547215451902604</v>
       </c>
     </row>
     <row r="244">
@@ -20633,71 +20633,71 @@
         <v>170</v>
       </c>
       <c r="B244" t="n">
-        <v>0.3534715762620668</v>
+        <v>0.3542862696939056</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="n">
-        <v>178</v>
+        <v>220</v>
       </c>
       <c r="B245" t="n">
-        <v>0.3514420820892857</v>
+        <v>0.3526408856249907</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="n">
-        <v>220</v>
+        <v>178</v>
       </c>
       <c r="B246" t="n">
-        <v>0.3506996814738267</v>
+        <v>0.3522470107221434</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="n">
-        <v>228</v>
+        <v>168</v>
       </c>
       <c r="B247" t="n">
-        <v>0.3468629854882611</v>
+        <v>0.3479376266396085</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="n">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="B248" t="n">
-        <v>0.3466069451693615</v>
+        <v>0.3478833536532929</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="n">
-        <v>169</v>
+        <v>238</v>
       </c>
       <c r="B249" t="n">
-        <v>0.3463914722047747</v>
+        <v>0.3476003785870247</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="n">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B250" t="n">
-        <v>0.3462346840628964</v>
+        <v>0.3472133337823546</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="n">
-        <v>177</v>
+        <v>227</v>
       </c>
       <c r="B251" t="n">
-        <v>0.3440738313465347</v>
+        <v>0.3454693055525317</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="n">
-        <v>227</v>
+        <v>177</v>
       </c>
       <c r="B252" t="n">
-        <v>0.3435540414182167</v>
+        <v>0.3448889394752062</v>
       </c>
     </row>
     <row r="253">
@@ -20705,7 +20705,7 @@
         <v>176</v>
       </c>
       <c r="B253" t="n">
-        <v>0.3393742969265104</v>
+        <v>0.3410531798551416</v>
       </c>
     </row>
     <row r="254">
@@ -20713,7 +20713,7 @@
         <v>246</v>
       </c>
       <c r="B254" t="n">
-        <v>0.3335733674380217</v>
+        <v>0.3345833307604607</v>
       </c>
     </row>
     <row r="255">
@@ -20721,7 +20721,7 @@
         <v>235</v>
       </c>
       <c r="B255" t="n">
-        <v>0.3064392598882635</v>
+        <v>0.3082036008260451</v>
       </c>
     </row>
     <row r="256">
@@ -20729,7 +20729,7 @@
         <v>237</v>
       </c>
       <c r="B256" t="n">
-        <v>0.3041690005385008</v>
+        <v>0.3053032548591206</v>
       </c>
     </row>
     <row r="257">
@@ -20737,7 +20737,7 @@
         <v>236</v>
       </c>
       <c r="B257" t="n">
-        <v>0.3009016610292082</v>
+        <v>0.3020270349591974</v>
       </c>
     </row>
   </sheetData>

</xml_diff>